<commit_message>
Fixed case of SW110, SW210, SW310 columns in observed file.
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/SWIM/HudsonObserved.xlsx
+++ b/Tests/UnderReview/SWIM/HudsonObserved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hol353\Repos\ApsimX\Prototypes\SWIM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\SWIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AB307A-5A1A-4B75-8364-A5AFE209B8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE7B293-234C-4D85-A039-5DC1D7932F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="390" windowWidth="19090" windowHeight="14010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5870" yWindow="60" windowWidth="19730" windowHeight="13300" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedCrop" sheetId="2" r:id="rId1"/>
@@ -202,15 +202,6 @@
     <t>Cl(16)</t>
   </si>
   <si>
-    <t>sw110</t>
-  </si>
-  <si>
-    <t>sw210</t>
-  </si>
-  <si>
-    <t>sw310</t>
-  </si>
-  <si>
     <t>sw_dep()</t>
   </si>
   <si>
@@ -389,6 +380,15 @@
   </si>
   <si>
     <t>HudsonW1</t>
+  </si>
+  <si>
+    <t>SW110</t>
+  </si>
+  <si>
+    <t>SW210</t>
+  </si>
+  <si>
+    <t>SW310</t>
   </si>
 </sst>
 </file>
@@ -841,33 +841,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2">
         <v>34634</v>
@@ -882,7 +882,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2">
         <v>34898</v>
@@ -891,7 +891,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2">
         <v>34928</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2">
         <v>34988</v>
@@ -921,7 +921,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2">
         <v>35031</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2">
         <v>35286</v>
@@ -948,7 +948,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="2">
         <v>35304</v>
@@ -963,7 +963,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2">
         <v>35326</v>
@@ -978,7 +978,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2">
         <v>35347</v>
@@ -993,7 +993,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2">
         <v>35403</v>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B12" s="2">
         <v>35628</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B13" s="2">
         <v>35641</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B14" s="2">
         <v>35670</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" s="2">
         <v>35690</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B16" s="2">
         <v>35713</v>
@@ -1079,7 +1079,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B17" s="2">
         <v>35760</v>
@@ -1094,7 +1094,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2">
         <v>36389</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B19" s="2">
         <v>36454</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B20" s="2">
         <v>36502</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B21" s="2">
         <v>36034</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2">
         <v>36052</v>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B23" s="2">
         <v>36066</v>
@@ -1187,7 +1187,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2">
         <v>36081</v>
@@ -1201,7 +1201,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25" s="2">
         <v>36131</v>
@@ -1218,7 +1218,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2">
         <v>36418</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B27" s="2">
         <v>36431</v>
@@ -1266,66 +1266,66 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>58</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>62</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>63</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>64</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>65</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>66</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>67</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>68</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="3">
         <v>34552</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="3">
         <v>34802</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="3">
         <v>35050</v>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" s="3">
         <v>35178</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="3">
         <v>35422</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" s="3">
         <v>35437</v>
@@ -1692,8 +1692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1705,19 +1705,19 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2">
         <v>34578</v>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2">
         <v>34790</v>
@@ -1906,7 +1906,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2">
         <v>35004</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2">
         <v>35156</v>
@@ -2042,7 +2042,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2">
         <v>35370</v>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2">
         <v>35521</v>
@@ -2178,7 +2178,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="2">
         <v>35735</v>
@@ -2246,7 +2246,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2">
         <v>35916</v>
@@ -2314,7 +2314,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2">
         <v>36100</v>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2">
         <v>36312</v>
@@ -2450,7 +2450,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B12" s="2">
         <v>36465</v>
@@ -2518,7 +2518,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B13" s="2">
         <v>36647</v>
@@ -2605,18 +2605,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2">
         <v>34634</v>
@@ -2627,7 +2627,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2">
         <v>34928</v>
@@ -2638,7 +2638,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2">
         <v>34988</v>
@@ -2649,7 +2649,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2">
         <v>35031</v>
@@ -2660,7 +2660,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2">
         <v>35304</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2">
         <v>35326</v>
@@ -2682,7 +2682,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="2">
         <v>35347</v>
@@ -2693,7 +2693,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2">
         <v>35403</v>
@@ -2704,7 +2704,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2">
         <v>35641</v>
@@ -2715,7 +2715,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2">
         <v>35670</v>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B12" s="2">
         <v>35690</v>
@@ -2737,7 +2737,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B13" s="2">
         <v>35713</v>
@@ -2748,7 +2748,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B14" s="2">
         <v>35760</v>
@@ -2759,7 +2759,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" s="2">
         <v>36034</v>
@@ -2770,7 +2770,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B16" s="2">
         <v>36052</v>
@@ -2781,7 +2781,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B17" s="2">
         <v>36066</v>
@@ -2792,7 +2792,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2">
         <v>36081</v>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B19" s="2">
         <v>36131</v>
@@ -2814,7 +2814,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B20" s="2">
         <v>36389</v>
@@ -2825,7 +2825,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B21" s="2">
         <v>36418</v>
@@ -2836,7 +2836,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2">
         <v>36431</v>
@@ -2847,7 +2847,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B23" s="2">
         <v>36454</v>
@@ -2858,7 +2858,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2">
         <v>36502</v>
@@ -2888,18 +2888,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2">
         <v>35657</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2">
         <v>35892</v>
@@ -2921,7 +2921,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2">
         <v>36026</v>
@@ -2932,7 +2932,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2">
         <v>36229</v>
@@ -2961,21 +2961,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2">
         <v>35307</v>
@@ -2989,7 +2989,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2">
         <v>35344</v>
@@ -3003,7 +3003,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2">
         <v>35405</v>
@@ -3017,7 +3017,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2">
         <v>35406</v>
@@ -3031,7 +3031,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2">
         <v>35459</v>
@@ -3045,7 +3045,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2">
         <v>35460</v>
@@ -3059,7 +3059,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="2">
         <v>35474</v>
@@ -3073,7 +3073,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2">
         <v>35834</v>
@@ -3087,7 +3087,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2">
         <v>35948</v>
@@ -3101,7 +3101,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2">
         <v>35968</v>
@@ -3115,7 +3115,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B12" s="2">
         <v>35994</v>
@@ -3129,7 +3129,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B13" s="2">
         <v>35996</v>
@@ -3143,7 +3143,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B14" s="2">
         <v>35997</v>
@@ -3157,7 +3157,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" s="2">
         <v>36000</v>
@@ -3171,7 +3171,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B16" s="2">
         <v>36002</v>
@@ -3185,7 +3185,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B17" s="2">
         <v>36003</v>
@@ -3199,7 +3199,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2">
         <v>36014</v>
@@ -3213,7 +3213,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B19" s="2">
         <v>36015</v>
@@ -3227,7 +3227,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B20" s="2">
         <v>36043</v>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B21" s="2">
         <v>36050</v>
@@ -3255,7 +3255,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2">
         <v>36051</v>
@@ -3269,7 +3269,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B23" s="2">
         <v>36052</v>
@@ -3283,7 +3283,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2">
         <v>36053</v>
@@ -3297,7 +3297,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25" s="2">
         <v>36056</v>
@@ -3311,7 +3311,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2">
         <v>36062</v>
@@ -3325,7 +3325,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B27" s="2">
         <v>36074</v>
@@ -3339,7 +3339,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B28" s="2">
         <v>36087</v>
@@ -3353,7 +3353,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B29" s="2">
         <v>36088</v>
@@ -3367,7 +3367,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B30" s="2">
         <v>36093</v>
@@ -3381,7 +3381,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B31" s="2">
         <v>36094</v>
@@ -3395,7 +3395,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B32" s="2">
         <v>36095</v>
@@ -3409,7 +3409,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B33" s="2">
         <v>36097</v>
@@ -3423,7 +3423,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B34" s="2">
         <v>36098</v>
@@ -3437,7 +3437,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B35" s="2">
         <v>36099</v>
@@ -3451,7 +3451,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B36" s="2">
         <v>36105</v>
@@ -3465,7 +3465,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B37" s="2">
         <v>36106</v>
@@ -3479,7 +3479,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B38" s="2">
         <v>36107</v>
@@ -3493,7 +3493,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B39" s="2">
         <v>36108</v>
@@ -3507,7 +3507,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B40" s="2">
         <v>36111</v>
@@ -3521,7 +3521,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B41" s="2">
         <v>36112</v>
@@ -3535,7 +3535,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B42" s="2">
         <v>36113</v>
@@ -3549,7 +3549,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B43" s="2">
         <v>36116</v>
@@ -3563,7 +3563,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B44" s="2">
         <v>36117</v>
@@ -3577,7 +3577,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B45" s="2">
         <v>36143</v>
@@ -3591,7 +3591,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B46" s="2">
         <v>36144</v>
@@ -3605,7 +3605,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B47" s="2">
         <v>36145</v>
@@ -3619,7 +3619,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B48" s="2">
         <v>36146</v>
@@ -3633,7 +3633,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B49" s="2">
         <v>36147</v>
@@ -3647,7 +3647,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B50" s="2">
         <v>36149</v>
@@ -3661,7 +3661,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B51" s="2">
         <v>36160</v>
@@ -3675,7 +3675,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B52" s="2">
         <v>36162</v>
@@ -3689,7 +3689,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B53" s="2">
         <v>36166</v>
@@ -3703,7 +3703,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B54" s="2">
         <v>36168</v>
@@ -3717,7 +3717,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B55" s="2">
         <v>36169</v>
@@ -3731,7 +3731,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B56" s="2">
         <v>36170</v>
@@ -3745,7 +3745,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B57" s="2">
         <v>36171</v>
@@ -3759,7 +3759,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B58" s="2">
         <v>36173</v>
@@ -3773,7 +3773,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B59" s="2">
         <v>36181</v>
@@ -3787,7 +3787,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B60" s="2">
         <v>36183</v>
@@ -3801,7 +3801,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B61" s="2">
         <v>36184</v>
@@ -3815,7 +3815,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B62" s="2">
         <v>36191</v>
@@ -3829,7 +3829,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B63" s="2">
         <v>36192</v>
@@ -3843,7 +3843,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B64" s="2">
         <v>36199</v>
@@ -3857,7 +3857,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B65" s="2">
         <v>36200</v>
@@ -3871,7 +3871,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B66" s="2">
         <v>36219</v>
@@ -3885,7 +3885,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B67" s="2">
         <v>36220</v>
@@ -3899,7 +3899,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B68" s="2">
         <v>36221</v>
@@ -3913,7 +3913,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B69" s="2">
         <v>36237</v>
@@ -3927,7 +3927,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B70" s="2">
         <v>36241</v>
@@ -3941,7 +3941,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B71" s="2">
         <v>36243</v>
@@ -3955,7 +3955,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B72" s="2">
         <v>36245</v>
@@ -3969,7 +3969,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B73" s="2">
         <v>36250</v>
@@ -3983,7 +3983,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B74" s="2">
         <v>36251</v>
@@ -3997,7 +3997,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B75" s="2">
         <v>36252</v>
@@ -4011,7 +4011,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B76" s="2">
         <v>36253</v>
@@ -4025,7 +4025,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B77" s="2">
         <v>36254</v>
@@ -4039,7 +4039,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B78" s="2">
         <v>36255</v>
@@ -4053,7 +4053,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B79" s="2">
         <v>36256</v>
@@ -4067,7 +4067,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B80" s="2">
         <v>36259</v>
@@ -4081,7 +4081,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B81" s="2">
         <v>36261</v>
@@ -4095,7 +4095,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B82" s="2">
         <v>36293</v>
@@ -4109,7 +4109,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B83" s="2">
         <v>36310</v>
@@ -4123,7 +4123,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B84" s="2">
         <v>36311</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B85" s="2">
         <v>36317</v>
@@ -4151,7 +4151,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B86" s="2">
         <v>36318</v>
@@ -4165,7 +4165,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B87" s="2">
         <v>36319</v>
@@ -4179,7 +4179,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B88" s="2">
         <v>36320</v>
@@ -4193,7 +4193,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B89" s="2">
         <v>36321</v>
@@ -4207,7 +4207,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B90" s="2">
         <v>36324</v>
@@ -4221,7 +4221,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B91" s="2">
         <v>36325</v>
@@ -4235,7 +4235,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B92" s="2">
         <v>36327</v>
@@ -4249,7 +4249,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B93" s="2">
         <v>36328</v>
@@ -4263,7 +4263,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B94" s="2">
         <v>36329</v>
@@ -4277,7 +4277,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B95" s="2">
         <v>36333</v>
@@ -4291,7 +4291,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B96" s="2">
         <v>36341</v>
@@ -4305,7 +4305,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B97" s="2">
         <v>36342</v>
@@ -4319,7 +4319,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B98" s="2">
         <v>36346</v>
@@ -4333,7 +4333,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B99" s="2">
         <v>36350</v>
@@ -4347,7 +4347,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B100" s="2">
         <v>36412</v>
@@ -4361,7 +4361,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B101" s="2">
         <v>36413</v>
@@ -4375,7 +4375,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B102" s="2">
         <v>36419</v>
@@ -4389,7 +4389,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B103" s="2">
         <v>36420</v>
@@ -4403,7 +4403,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B104" s="2">
         <v>36428</v>
@@ -4417,7 +4417,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B105" s="2">
         <v>36429</v>
@@ -4431,7 +4431,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B106" s="2">
         <v>36431</v>
@@ -4445,7 +4445,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B107" s="2">
         <v>36433</v>
@@ -4459,7 +4459,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B108" s="2">
         <v>36435</v>
@@ -4473,7 +4473,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B109" s="2">
         <v>36436</v>
@@ -4487,7 +4487,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B110" s="2">
         <v>36437</v>
@@ -4501,7 +4501,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B111" s="2">
         <v>36438</v>
@@ -4515,7 +4515,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B112" s="2">
         <v>36440</v>
@@ -4529,7 +4529,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B113" s="2">
         <v>36441</v>
@@ -4543,7 +4543,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B114" s="2">
         <v>36443</v>
@@ -4557,7 +4557,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B115" s="2">
         <v>36444</v>
@@ -4571,7 +4571,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B116" s="2">
         <v>36447</v>
@@ -4585,7 +4585,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B117" s="2">
         <v>36448</v>
@@ -4599,7 +4599,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B118" s="2">
         <v>36451</v>
@@ -4613,7 +4613,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B119" s="2">
         <v>36452</v>
@@ -4627,7 +4627,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B120" s="2">
         <v>36454</v>
@@ -4641,7 +4641,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B121" s="2">
         <v>36455</v>
@@ -4655,7 +4655,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B122" s="2">
         <v>36456</v>
@@ -4669,7 +4669,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B123" s="2">
         <v>36457</v>
@@ -4683,7 +4683,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B124" s="2">
         <v>36458</v>
@@ -4697,7 +4697,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B125" s="2">
         <v>36463</v>
@@ -4711,7 +4711,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B126" s="2">
         <v>36464</v>
@@ -4725,7 +4725,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B127" s="2">
         <v>36465</v>
@@ -4739,7 +4739,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B128" s="2">
         <v>36469</v>
@@ -4753,7 +4753,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B129" s="2">
         <v>36470</v>
@@ -4767,7 +4767,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B130" s="2">
         <v>36471</v>
@@ -4781,7 +4781,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B131" s="2">
         <v>36472</v>
@@ -4795,7 +4795,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B132" s="2">
         <v>36474</v>
@@ -4809,7 +4809,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B133" s="2">
         <v>36476</v>
@@ -4823,7 +4823,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B134" s="2">
         <v>36479</v>
@@ -4837,7 +4837,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B135" s="2">
         <v>36480</v>
@@ -4851,7 +4851,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B136" s="2">
         <v>36481</v>
@@ -4865,7 +4865,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B137" s="2">
         <v>36482</v>
@@ -4879,7 +4879,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B138" s="2">
         <v>36485</v>
@@ -4893,7 +4893,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B139" s="2">
         <v>36490</v>
@@ -4907,7 +4907,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B140" s="2">
         <v>36498</v>
@@ -4921,7 +4921,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B141" s="2">
         <v>36503</v>
@@ -4935,7 +4935,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B142" s="2">
         <v>36504</v>
@@ -4949,7 +4949,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B143" s="2">
         <v>36505</v>
@@ -4963,7 +4963,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B144" s="2">
         <v>36511</v>
@@ -4977,7 +4977,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B145" s="2">
         <v>36517</v>
@@ -4991,7 +4991,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B146" s="2">
         <v>36518</v>
@@ -5005,7 +5005,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B147" s="2">
         <v>36519</v>
@@ -5019,7 +5019,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B148" s="2">
         <v>36520</v>
@@ -5033,7 +5033,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B149" s="2">
         <v>36521</v>
@@ -5047,7 +5047,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B150" s="2">
         <v>36522</v>
@@ -5061,7 +5061,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B151" s="2">
         <v>36523</v>
@@ -5075,7 +5075,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B152" s="2">
         <v>36524</v>
@@ -5089,7 +5089,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B153" s="2">
         <v>36528</v>
@@ -5103,7 +5103,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B154" s="2">
         <v>36529</v>
@@ -5136,18 +5136,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2">
         <v>35657</v>
@@ -5158,7 +5158,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2">
         <v>35892</v>
@@ -5169,7 +5169,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2">
         <v>36026</v>
@@ -5180,7 +5180,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2">
         <v>36229</v>
@@ -5198,8 +5198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5210,27 +5210,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2">
         <v>34690</v>
@@ -5250,7 +5250,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2">
         <v>34876</v>
@@ -5270,7 +5270,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2">
         <v>34905</v>
@@ -5290,7 +5290,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2">
         <v>34941</v>
@@ -5310,7 +5310,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2">
         <v>34969</v>
@@ -5330,7 +5330,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2">
         <v>35004</v>
@@ -5350,7 +5350,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="2">
         <v>35033</v>
@@ -5370,7 +5370,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2">
         <v>35074</v>
@@ -5390,7 +5390,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2">
         <v>35104</v>
@@ -5410,7 +5410,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2">
         <v>35131</v>
@@ -5430,7 +5430,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B12" s="2">
         <v>35153</v>
@@ -5450,7 +5450,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B13" s="2">
         <v>35200</v>
@@ -5470,7 +5470,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B14" s="2">
         <v>35224</v>
@@ -5490,7 +5490,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" s="2">
         <v>35257</v>
@@ -5510,7 +5510,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B16" s="2">
         <v>35298</v>
@@ -5530,7 +5530,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B17" s="2">
         <v>35328</v>
@@ -5550,7 +5550,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2">
         <v>35362</v>
@@ -5570,7 +5570,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B19" s="2">
         <v>35404</v>
@@ -5590,7 +5590,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B20" s="2">
         <v>35443</v>
@@ -5610,7 +5610,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B21" s="2">
         <v>35467</v>
@@ -5630,7 +5630,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2">
         <v>35482</v>
@@ -5650,7 +5650,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B23" s="2">
         <v>35503</v>
@@ -5670,7 +5670,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2">
         <v>35542</v>
@@ -5690,7 +5690,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25" s="2">
         <v>35579</v>
@@ -5710,7 +5710,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2">
         <v>35605</v>
@@ -5730,7 +5730,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B27" s="2">
         <v>35634</v>
@@ -5750,7 +5750,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B28" s="2">
         <v>35669</v>
@@ -5770,7 +5770,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B29" s="2">
         <v>35702</v>
@@ -5790,7 +5790,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B30" s="2">
         <v>35726</v>
@@ -5810,7 +5810,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B31" s="2">
         <v>35768</v>
@@ -5830,7 +5830,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B32" s="2">
         <v>35786</v>
@@ -5850,7 +5850,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B33" s="2">
         <v>35815</v>
@@ -5870,7 +5870,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B34" s="2">
         <v>35850</v>
@@ -5890,7 +5890,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B35" s="2">
         <v>35879</v>
@@ -5910,7 +5910,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B36" s="2">
         <v>35913</v>
@@ -5930,7 +5930,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B37" s="2">
         <v>35940</v>
@@ -5950,7 +5950,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B38" s="2">
         <v>35956</v>
@@ -5970,7 +5970,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B39" s="2">
         <v>35979</v>
@@ -5990,7 +5990,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B40" s="2">
         <v>36007</v>
@@ -6010,7 +6010,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B41" s="2">
         <v>36039</v>
@@ -6030,7 +6030,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B42" s="2">
         <v>34852</v>
@@ -6050,7 +6050,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B43" s="2">
         <v>36061</v>
@@ -6070,7 +6070,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B44" s="2">
         <v>36089</v>
@@ -6090,7 +6090,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B45" s="2">
         <v>36137</v>
@@ -6110,7 +6110,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B46" s="2">
         <v>36151</v>
@@ -6130,7 +6130,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B47" s="2">
         <v>36185</v>
@@ -6150,7 +6150,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B48" s="2">
         <v>36216</v>
@@ -6170,7 +6170,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B49" s="2">
         <v>36237</v>
@@ -6190,7 +6190,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B50" s="2">
         <v>36273</v>
@@ -6210,7 +6210,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B51" s="2">
         <v>36305</v>
@@ -6230,7 +6230,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B52" s="2">
         <v>36341</v>
@@ -6250,7 +6250,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B53" s="2">
         <v>36369</v>
@@ -6270,7 +6270,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B54" s="2">
         <v>36398</v>
@@ -6290,7 +6290,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B55" s="2">
         <v>36405</v>
@@ -6310,7 +6310,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B56" s="2">
         <v>36426</v>
@@ -6330,7 +6330,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B57" s="2">
         <v>36454</v>
@@ -6350,7 +6350,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B58" s="2">
         <v>36482</v>
@@ -6370,7 +6370,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B59" s="2">
         <v>36507</v>
@@ -6390,7 +6390,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B60" s="2">
         <v>36545</v>
@@ -6434,57 +6434,57 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>30</v>
-      </c>
-      <c r="N1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2">
         <v>34690</v>
@@ -6534,7 +6534,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2">
         <v>34852</v>
@@ -6584,7 +6584,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2">
         <v>34876</v>
@@ -6634,7 +6634,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2">
         <v>34905</v>
@@ -6684,7 +6684,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2">
         <v>34941</v>
@@ -6734,7 +6734,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2">
         <v>34969</v>
@@ -6784,7 +6784,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="2">
         <v>35004</v>
@@ -6834,7 +6834,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2">
         <v>35033</v>
@@ -6884,7 +6884,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2">
         <v>35074</v>
@@ -6934,7 +6934,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2">
         <v>35104</v>
@@ -6984,7 +6984,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B12" s="2">
         <v>35131</v>
@@ -7034,7 +7034,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B13" s="2">
         <v>35153</v>
@@ -7084,7 +7084,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B14" s="2">
         <v>35200</v>
@@ -7134,7 +7134,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" s="2">
         <v>35224</v>
@@ -7184,7 +7184,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B16" s="2">
         <v>35257</v>
@@ -7234,7 +7234,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B17" s="2">
         <v>35298</v>
@@ -7284,7 +7284,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2">
         <v>35328</v>
@@ -7334,7 +7334,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B19" s="2">
         <v>35362</v>
@@ -7384,7 +7384,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B20" s="2">
         <v>35404</v>
@@ -7434,7 +7434,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B21" s="2">
         <v>35443</v>
@@ -7484,7 +7484,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2">
         <v>35467</v>
@@ -7534,7 +7534,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B23" s="2">
         <v>35482</v>
@@ -7584,7 +7584,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2">
         <v>35503</v>
@@ -7634,7 +7634,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25" s="2">
         <v>35542</v>
@@ -7684,7 +7684,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2">
         <v>35579</v>
@@ -7734,7 +7734,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B27" s="2">
         <v>35605</v>
@@ -7784,7 +7784,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B28" s="2">
         <v>35634</v>
@@ -7834,7 +7834,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B29" s="2">
         <v>35669</v>
@@ -7884,7 +7884,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B30" s="2">
         <v>35702</v>
@@ -7934,7 +7934,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B31" s="2">
         <v>35726</v>
@@ -7984,7 +7984,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B32" s="2">
         <v>35768</v>
@@ -8034,7 +8034,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B33" s="2">
         <v>35786</v>
@@ -8084,7 +8084,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B34" s="2">
         <v>35815</v>
@@ -8134,7 +8134,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B35" s="2">
         <v>35850</v>
@@ -8184,7 +8184,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B36" s="2">
         <v>35879</v>
@@ -8234,7 +8234,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B37" s="2">
         <v>35913</v>
@@ -8284,7 +8284,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B38" s="2">
         <v>35940</v>
@@ -8334,7 +8334,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B39" s="2">
         <v>35956</v>
@@ -8384,7 +8384,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B40" s="2">
         <v>35979</v>
@@ -8434,7 +8434,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B41" s="2">
         <v>36007</v>
@@ -8484,7 +8484,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B42" s="2">
         <v>36039</v>
@@ -8534,7 +8534,7 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B43" s="2">
         <v>36061</v>
@@ -8584,7 +8584,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B44" s="2">
         <v>36089</v>
@@ -8634,7 +8634,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B45" s="2">
         <v>36137</v>
@@ -8684,7 +8684,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B46" s="2">
         <v>36151</v>
@@ -8734,7 +8734,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B47" s="2">
         <v>36185</v>
@@ -8784,7 +8784,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B48" s="2">
         <v>36216</v>
@@ -8834,7 +8834,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B49" s="2">
         <v>36237</v>
@@ -8884,7 +8884,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B50" s="2">
         <v>36273</v>
@@ -8934,7 +8934,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B51" s="2">
         <v>36305</v>
@@ -8984,7 +8984,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B52" s="2">
         <v>36341</v>
@@ -9034,7 +9034,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B53" s="2">
         <v>36369</v>
@@ -9084,7 +9084,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B54" s="2">
         <v>36398</v>
@@ -9134,7 +9134,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B55" s="2">
         <v>36405</v>
@@ -9184,7 +9184,7 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B56" s="2">
         <v>36426</v>
@@ -9234,7 +9234,7 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B57" s="2">
         <v>36454</v>
@@ -9284,7 +9284,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B58" s="2">
         <v>36482</v>
@@ -9334,7 +9334,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B59" s="2">
         <v>36507</v>
@@ -9384,7 +9384,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B60" s="2">
         <v>36545</v>
@@ -9460,45 +9460,45 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" t="s">
-        <v>54</v>
-      </c>
       <c r="K1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2">
         <v>34574</v>
@@ -9542,7 +9542,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2">
         <v>34999</v>
@@ -9586,7 +9586,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2">
         <v>35152</v>
@@ -9630,7 +9630,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2">
         <v>35361</v>
@@ -9674,7 +9674,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2">
         <v>35514</v>
@@ -9718,7 +9718,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2">
         <v>35729</v>
@@ -9762,7 +9762,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="2">
         <v>35910</v>
@@ -9806,7 +9806,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2">
         <v>36093</v>
@@ -9850,7 +9850,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2">
         <v>36307</v>
@@ -9894,7 +9894,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2">
         <v>36461</v>
@@ -9938,7 +9938,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B12" s="2">
         <v>36642</v>
@@ -9982,7 +9982,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B13" s="2">
         <v>34574</v>
@@ -10026,7 +10026,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B14" s="2">
         <v>34999</v>
@@ -10070,7 +10070,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B15" s="2">
         <v>35152</v>
@@ -10114,7 +10114,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B16" s="2">
         <v>35361</v>
@@ -10158,7 +10158,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B17" s="2">
         <v>35514</v>
@@ -10202,7 +10202,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B18" s="2">
         <v>35729</v>
@@ -10246,7 +10246,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B19" s="2">
         <v>35910</v>
@@ -10290,7 +10290,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B20" s="2">
         <v>36093</v>
@@ -10334,7 +10334,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B21" s="2">
         <v>36307</v>
@@ -10378,7 +10378,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B22" s="2">
         <v>36461</v>
@@ -10422,7 +10422,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B23" s="2">
         <v>36642</v>

</xml_diff>